<commit_message>
1. Added Automate WIth Rakesh LINQ Folder And Sequences. 2. Added Input Excel Files. 3. Completed LINQ Exercises provided by Rakesh 4. Add Differences between Double, and Decimal.
</commit_message>
<xml_diff>
--- a/Input/Employee_Salary_Details.xlsx
+++ b/Input/Employee_Salary_Details.xlsx
@@ -4,13 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="683" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet19" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet20" sheetId="8" r:id="rId3"/>
+    <sheet name="Sheet26" sheetId="10" r:id="rId4"/>
+    <sheet name="Sheet25" sheetId="9" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet33" sheetId="11" r:id="rId7"/>
+    <sheet name="Sheet15" sheetId="6" r:id="rId8"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId9"/>
+    <sheet name="Sheet3" sheetId="2" r:id="rId10"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="12">
   <si>
     <t>Dept</t>
   </si>
@@ -436,110 +443,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>10001</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>10002</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>10003</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>10004</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>10005</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>20000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -582,7 +490,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -625,4 +533,497 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10005</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>20000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10004</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>15000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>40000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10002</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10004</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>15000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10005</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>20000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10005</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>20000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10005</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>20000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>